<commit_message>
SoC version: Passes fabrication in JLCPCB
</commit_message>
<xml_diff>
--- a/v7-soc-8bit/fabrication/v7-soc-8bit-all-pos.xlsx
+++ b/v7-soc-8bit/fabrication/v7-soc-8bit-all-pos.xlsx
@@ -235,10 +235,10 @@
         </is>
       </c>
       <c r="B6" s="3">
-        <v>78.959999999999994</v>
+        <v>78.799999999999997</v>
       </c>
       <c r="C6" s="3">
-        <v>-38.960000000000001</v>
+        <v>-38.950000000000003</v>
       </c>
       <c r="D6" s="3">
         <v>-90</v>
@@ -254,10 +254,10 @@
         </is>
       </c>
       <c r="B7" s="3">
-        <v>77.200000000000003</v>
+        <v>77.290000000000006</v>
       </c>
       <c r="C7" s="3">
-        <v>-42.090000000000003</v>
+        <v>-42.280000000000001</v>
       </c>
       <c r="D7" s="3">
         <v>-90</v>
@@ -273,10 +273,10 @@
         </is>
       </c>
       <c r="B8" s="3">
-        <v>80.625</v>
+        <v>80.590000000000003</v>
       </c>
       <c r="C8" s="3">
-        <v>-42.090000000000003</v>
+        <v>-42.280000000000001</v>
       </c>
       <c r="D8" s="3">
         <v>90</v>
@@ -577,10 +577,10 @@
         </is>
       </c>
       <c r="B24" s="3">
-        <v>78.950000000000003</v>
+        <v>78.939999999999998</v>
       </c>
       <c r="C24" s="3">
-        <v>-42.090000000000003</v>
+        <v>-42.280000000000001</v>
       </c>
       <c r="D24" s="3">
         <v>-90</v>
@@ -767,10 +767,10 @@
         </is>
       </c>
       <c r="B34" s="3">
-        <v>63.575800000000001</v>
+        <v>63.68</v>
       </c>
       <c r="C34" s="3">
-        <v>-49.779998999999997</v>
+        <v>-49.770000000000003</v>
       </c>
       <c r="D34" s="3">
         <v>0</v>

</xml_diff>